<commit_message>
Added support for mounts with different gear ratio on each axis. For those with the same gear ratio on each mount, this update doesn't affect you.
</commit_message>
<xml_diff>
--- a/AstroEQ5/Open me first/Initialisation Variable Calculator.xlsx
+++ b/AstroEQ5/Open me first/Initialisation Variable Calculator.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>divisor</t>
   </si>
@@ -39,12 +39,6 @@
     <t>Error (s)</t>
   </si>
   <si>
-    <t>aVal</t>
-  </si>
-  <si>
-    <t>bVal</t>
-  </si>
-  <si>
     <t>Scalar</t>
   </si>
   <si>
@@ -63,9 +57,6 @@
     <t>Worm Teeth</t>
   </si>
   <si>
-    <t>sVal</t>
-  </si>
-  <si>
     <t>Step Angle (deg)</t>
   </si>
   <si>
@@ -109,6 +100,33 @@
   </si>
   <si>
     <t>This can be used as an alternative to the "step angle" cell if you know the steps per rotation rather than the angle. (Note, the content of the Step Angle cell will be ignored if this is not 0)</t>
+  </si>
+  <si>
+    <t>aVal1</t>
+  </si>
+  <si>
+    <t>aVal2</t>
+  </si>
+  <si>
+    <t>bVal2</t>
+  </si>
+  <si>
+    <t>bVal1</t>
+  </si>
+  <si>
+    <t>sVal1</t>
+  </si>
+  <si>
+    <t>sVal2</t>
+  </si>
+  <si>
+    <t>Use Different Ratio?</t>
+  </si>
+  <si>
+    <t>If your mount has a different gear ratio for each axis, then set this to a 1. Then set the RA axis values above, and DEC axis values below.</t>
+  </si>
+  <si>
+    <t>Use the values below to set the DEC axis specific values only if your mount has a different ratio for each axis. If this is the case, also remember to set the "Use Different Ratio?" box to be a 1</t>
   </si>
 </sst>
 </file>
@@ -118,7 +136,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,6 +198,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -237,7 +263,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -457,11 +483,92 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -533,39 +640,6 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -585,6 +659,93 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -915,10 +1076,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:S23"/>
+  <dimension ref="A1:S48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -945,40 +1106,40 @@
   <sheetData>
     <row r="1" spans="2:19" ht="15.75" thickBot="1">
       <c r="B1" s="27" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="11" t="s">
-        <v>11</v>
-      </c>
       <c r="O1" s="12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="2:19" ht="15.75" thickBot="1">
@@ -1013,7 +1174,7 @@
         <v>62667</v>
       </c>
       <c r="M2" s="15">
-        <f>IF(G2=0,ROUNDUP(I2/10000000,0),G2)</f>
+        <f>IF(G2=0,ROUNDUP(I2/10000000,0),IF(G2&lt;ROUNDUP(I2/10000000,0),ROUNDUP(I2/10000000,0),G2))</f>
         <v>1</v>
       </c>
       <c r="N2" s="13">
@@ -1025,46 +1186,46 @@
       </c>
     </row>
     <row r="3" spans="2:19" ht="15" customHeight="1">
-      <c r="B3" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="G3" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
+      <c r="B3" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="G3" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
     </row>
     <row r="4" spans="2:19" ht="15.75" thickBot="1">
-      <c r="B4" s="45"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="G4" s="36"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="G4" s="43"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="46"/>
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
       <c r="R4" s="9"/>
     </row>
-    <row r="5" spans="2:19" ht="15.75" hidden="1" customHeight="1" thickBot="1">
-      <c r="B5" s="45"/>
+    <row r="5" spans="2:19" ht="15.75" hidden="1" customHeight="1">
+      <c r="B5" s="34"/>
       <c r="I5">
         <f>K2</f>
         <v>64933</v>
@@ -1073,8 +1234,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:19" ht="15.75" hidden="1" customHeight="1" thickBot="1">
-      <c r="B6" s="45"/>
+    <row r="6" spans="2:19" ht="15.75" hidden="1" customHeight="1">
+      <c r="B6" s="34"/>
       <c r="I6">
         <f>N2*O2</f>
         <v>124000000</v>
@@ -1095,10 +1256,10 @@
         <v>19096</v>
       </c>
     </row>
-    <row r="7" spans="2:19" ht="15.75" hidden="1" customHeight="1" thickBot="1">
-      <c r="B7" s="45"/>
+    <row r="7" spans="2:19" ht="15.75" hidden="1" customHeight="1">
+      <c r="B7" s="34"/>
       <c r="I7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J7" t="s">
         <v>2</v>
@@ -1116,8 +1277,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="2:19" ht="15.75" hidden="1" customHeight="1" thickBot="1">
-      <c r="B8" s="45"/>
+    <row r="8" spans="2:19" ht="15.75" hidden="1" customHeight="1">
+      <c r="B8" s="34"/>
       <c r="I8" t="str">
         <f>CONCATENATE(" ",I2,",")</f>
         <v xml:space="preserve"> 9024000,</v>
@@ -1142,81 +1303,88 @@
         <v>38.865415120200794</v>
       </c>
     </row>
-    <row r="9" spans="2:19" ht="15.75" hidden="1" customHeight="1" thickBot="1">
-      <c r="B9" s="45"/>
+    <row r="9" spans="2:19" ht="15.75" hidden="1" customHeight="1">
+      <c r="B9" s="34"/>
       <c r="I9" s="2" t="str">
         <f>CONCATENATE(" ",K2,",")</f>
         <v xml:space="preserve"> 64933,</v>
       </c>
     </row>
-    <row r="10" spans="2:19" ht="15.75" hidden="1" customHeight="1" thickBot="1">
-      <c r="B10" s="45"/>
+    <row r="10" spans="2:19" ht="15.75" hidden="1" customHeight="1">
+      <c r="B10" s="34"/>
       <c r="I10" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="2:19" ht="15.75" hidden="1" customHeight="1" thickBot="1">
-      <c r="B11" s="45"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" ht="15.75" hidden="1" customHeight="1">
+      <c r="B11" s="34"/>
       <c r="I11" s="2" t="str">
         <f>CONCATENATE(" ",L2,",")</f>
         <v xml:space="preserve"> 62667,</v>
       </c>
     </row>
     <row r="12" spans="2:19" ht="15.75" hidden="1" customHeight="1" thickBot="1">
-      <c r="B12" s="45"/>
+      <c r="B12" s="34"/>
       <c r="I12" s="2" t="str">
         <f>CONCATENATE(" ",M2,");")</f>
         <v xml:space="preserve"> 1);</v>
       </c>
     </row>
     <row r="13" spans="2:19" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="B13" s="45"/>
-      <c r="C13" s="30" t="s">
+      <c r="B13" s="34"/>
+      <c r="C13" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="37"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="36" t="str">
+        <f>IF(E16,CONCATENATE("Synta synta(",I7,I8,I29,I9,I30,I11,I31,I10,I12),CONCATENATE("Synta synta(",I7,I8,I9,I10,I11,I12))</f>
+        <v>Synta synta(1281, 9024000, 64933, 16, 62667, 1);</v>
+      </c>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="38"/>
+    </row>
+    <row r="14" spans="2:19" ht="15.75" thickBot="1">
+      <c r="B14" s="34"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="41"/>
+    </row>
+    <row r="15" spans="2:19" ht="15.75" thickBot="1">
+      <c r="B15" s="34"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="2:19" ht="15.75" thickBot="1">
+      <c r="B16" s="34"/>
+      <c r="C16" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="54"/>
+      <c r="E16" s="59">
+        <v>0</v>
+      </c>
+      <c r="G16" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="29" t="str">
-        <f>CONCATENATE("Synta synta(",I7,I8,I9,I10,I11,I12)</f>
-        <v>Synta synta(1281, 9024000, 64933, 16, 62667, 1);</v>
-      </c>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
-    </row>
-    <row r="14" spans="2:19" ht="15.75" thickBot="1">
-      <c r="B14" s="45"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="34"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
-      <c r="O14" s="19"/>
-    </row>
-    <row r="15" spans="2:19">
-      <c r="B15" s="45"/>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="2:19">
-      <c r="B16" s="45"/>
-      <c r="G16" s="25" t="s">
-        <v>27</v>
-      </c>
       <c r="H16" s="20" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>4</v>
@@ -1228,13 +1396,18 @@
         <v>6</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12">
-      <c r="B17" s="45"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18">
+      <c r="B17" s="52"/>
+      <c r="C17" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
       <c r="G17" s="23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H17" s="22"/>
       <c r="I17">
@@ -1254,10 +1427,13 @@
         <v>-3.0116954579833508E-4</v>
       </c>
     </row>
-    <row r="18" spans="2:12">
-      <c r="B18" s="45"/>
+    <row r="18" spans="2:18">
+      <c r="B18" s="34"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="58"/>
       <c r="G18" s="24" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H18" s="21"/>
       <c r="I18">
@@ -1277,32 +1453,348 @@
         <v>-3.4103534116730933E-3</v>
       </c>
     </row>
-    <row r="19" spans="2:12">
-      <c r="B19" s="46"/>
-    </row>
-    <row r="20" spans="2:12">
-      <c r="B20" s="42"/>
-    </row>
-    <row r="21" spans="2:12">
-      <c r="B21" s="42"/>
-    </row>
-    <row r="22" spans="2:12">
-      <c r="B22" s="42"/>
-      <c r="L22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12">
-      <c r="B23" s="43"/>
+    <row r="19" spans="2:18">
+      <c r="B19" s="35"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
+    </row>
+    <row r="20" spans="2:18">
+      <c r="B20" s="51"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="51"/>
+      <c r="O20" s="51"/>
+    </row>
+    <row r="21" spans="2:18" ht="15.75" thickBot="1">
+      <c r="B21" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="61"/>
+      <c r="G21" s="61"/>
+      <c r="H21" s="61"/>
+      <c r="I21" s="61"/>
+      <c r="J21" s="61"/>
+      <c r="K21" s="61"/>
+      <c r="L21" s="61"/>
+      <c r="M21" s="61"/>
+      <c r="N21" s="61"/>
+      <c r="O21" s="61"/>
+    </row>
+    <row r="22" spans="2:18" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B22" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="47"/>
+      <c r="I22" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L22" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M22" s="10"/>
+      <c r="N22" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="O22" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" ht="15.75" thickBot="1">
+      <c r="B23" s="28">
+        <v>0</v>
+      </c>
+      <c r="C23" s="26">
+        <v>1.8</v>
+      </c>
+      <c r="D23" s="16">
+        <v>705</v>
+      </c>
+      <c r="E23" s="17">
+        <v>144</v>
+      </c>
+      <c r="G23" s="48"/>
+      <c r="I23" s="15">
+        <f>D23*IF(B23=0,(360/C23),B23)*64</f>
+        <v>9024000</v>
+      </c>
+      <c r="J23" s="13">
+        <v>86164.090500000006</v>
+      </c>
+      <c r="K23" s="15">
+        <f>ROUND(N23*I23/J23,0)</f>
+        <v>64933</v>
+      </c>
+      <c r="L23" s="15">
+        <f>ROUND(I23/E23,0)</f>
+        <v>62667</v>
+      </c>
+      <c r="M23" s="49"/>
+      <c r="N23" s="13">
+        <v>620</v>
+      </c>
+      <c r="O23" s="14">
+        <f>IF(K23&lt;160000,200000,1600000)</f>
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" ht="15" customHeight="1">
+      <c r="B24" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="G24" s="31"/>
+      <c r="I24" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="J24" s="46"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="46"/>
+      <c r="N24" s="46"/>
+      <c r="O24" s="46"/>
+    </row>
+    <row r="25" spans="2:18">
+      <c r="B25" s="34"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="G25" s="31"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="46"/>
+      <c r="N25" s="46"/>
+      <c r="O25" s="46"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+    </row>
+    <row r="26" spans="2:18" ht="15" hidden="1" customHeight="1">
+      <c r="B26" s="34"/>
+    </row>
+    <row r="27" spans="2:18" ht="15" hidden="1" customHeight="1">
+      <c r="B27" s="34"/>
+    </row>
+    <row r="28" spans="2:18" ht="15" hidden="1" customHeight="1">
+      <c r="B28" s="34"/>
+    </row>
+    <row r="29" spans="2:18" ht="15" hidden="1" customHeight="1">
+      <c r="B29" s="34"/>
+      <c r="I29" t="str">
+        <f>CONCATENATE(" ",I23,",")</f>
+        <v xml:space="preserve"> 9024000,</v>
+      </c>
+      <c r="R29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" ht="15" hidden="1" customHeight="1">
+      <c r="B30" s="34"/>
+      <c r="I30" s="2" t="str">
+        <f>CONCATENATE(" ",K23,",")</f>
+        <v xml:space="preserve"> 64933,</v>
+      </c>
+      <c r="J30" s="50"/>
+      <c r="K30" s="50"/>
+      <c r="L30" s="50"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+    </row>
+    <row r="31" spans="2:18" ht="15" hidden="1" customHeight="1">
+      <c r="B31" s="34"/>
+      <c r="I31" s="2" t="str">
+        <f>CONCATENATE(" ",L23,",")</f>
+        <v xml:space="preserve"> 62667,</v>
+      </c>
+      <c r="J31" s="50"/>
+      <c r="K31" s="50"/>
+      <c r="L31" s="50"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+    </row>
+    <row r="32" spans="2:18" ht="15" hidden="1" customHeight="1">
+      <c r="B32" s="34"/>
+    </row>
+    <row r="33" spans="1:15" ht="15" hidden="1" customHeight="1">
+      <c r="B33" s="34"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="47"/>
+      <c r="K33" s="47"/>
+      <c r="L33" s="47"/>
+      <c r="M33" s="32"/>
+      <c r="N33" s="32"/>
+      <c r="O33" s="32"/>
+    </row>
+    <row r="34" spans="1:15" ht="15" hidden="1" customHeight="1">
+      <c r="A34" s="9"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="50"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50"/>
+      <c r="G34" s="50"/>
+      <c r="H34" s="50"/>
+      <c r="I34" s="50"/>
+      <c r="J34" s="65"/>
+      <c r="K34" s="65"/>
+      <c r="L34" s="66"/>
+      <c r="M34" s="32"/>
+      <c r="N34" s="32"/>
+      <c r="O34" s="32"/>
+    </row>
+    <row r="35" spans="1:15" ht="15" hidden="1" customHeight="1">
+      <c r="B35" s="34"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="50"/>
+      <c r="J35" s="65"/>
+      <c r="K35" s="65"/>
+      <c r="L35" s="66"/>
+      <c r="M35" s="32"/>
+      <c r="N35" s="32"/>
+      <c r="O35" s="32"/>
+    </row>
+    <row r="36" spans="1:15" ht="15" hidden="1" customHeight="1">
+      <c r="B36" s="34"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="32"/>
+      <c r="L36" s="32"/>
+      <c r="M36" s="32"/>
+      <c r="N36" s="32"/>
+      <c r="O36" s="32"/>
+    </row>
+    <row r="37" spans="1:15" hidden="1">
+      <c r="B37" s="34"/>
+      <c r="G37" s="62"/>
+      <c r="H37" s="63"/>
+      <c r="I37" s="47"/>
+      <c r="J37" s="32"/>
+      <c r="K37" s="32"/>
+      <c r="L37" s="32"/>
+      <c r="M37" s="32"/>
+      <c r="N37" s="32"/>
+      <c r="O37" s="32"/>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="B38" s="34"/>
+      <c r="G38" s="64"/>
+      <c r="H38" s="64"/>
+      <c r="I38" s="32"/>
+      <c r="J38" s="32"/>
+      <c r="K38" s="32"/>
+      <c r="L38" s="32"/>
+      <c r="M38" s="32"/>
+      <c r="N38" s="32"/>
+      <c r="O38" s="32"/>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="B39" s="34"/>
+      <c r="G39" s="64"/>
+      <c r="H39" s="64"/>
+      <c r="I39" s="32"/>
+      <c r="J39" s="32"/>
+      <c r="K39" s="32"/>
+      <c r="L39" s="32"/>
+      <c r="M39" s="32"/>
+      <c r="N39" s="32"/>
+      <c r="O39" s="32"/>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="B40" s="34"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="32"/>
+      <c r="J40" s="32"/>
+      <c r="K40" s="32"/>
+      <c r="L40" s="32"/>
+      <c r="M40" s="32"/>
+      <c r="N40" s="32"/>
+      <c r="O40" s="32"/>
+    </row>
+    <row r="41" spans="1:15">
+      <c r="B41" s="34"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="32"/>
+      <c r="I41" s="32"/>
+    </row>
+    <row r="42" spans="1:15">
+      <c r="B42" s="34"/>
+      <c r="G42" s="32"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="32"/>
+    </row>
+    <row r="43" spans="1:15">
+      <c r="B43" s="34"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="32"/>
+    </row>
+    <row r="44" spans="1:15">
+      <c r="B44" s="35"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="32"/>
+    </row>
+    <row r="48" spans="1:15">
+      <c r="G48" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="G13:L14"/>
+  <mergeCells count="12">
+    <mergeCell ref="B21:O21"/>
+    <mergeCell ref="C24:E25"/>
+    <mergeCell ref="I24:O25"/>
+    <mergeCell ref="B24:B44"/>
+    <mergeCell ref="B3:B19"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="C3:E4"/>
     <mergeCell ref="I3:O4"/>
     <mergeCell ref="C13:E14"/>
-    <mergeCell ref="B3:B19"/>
+    <mergeCell ref="G13:O14"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added support for changing goto speed. Also added support for using the Pololu A4983 board rather than the DRV8824 chips.
</commit_message>
<xml_diff>
--- a/AstroEQ5/Open me first/Initialisation Variable Calculator.xlsx
+++ b/AstroEQ5/Open me first/Initialisation Variable Calculator.xlsx
@@ -568,7 +568,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -603,15 +603,6 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -631,13 +622,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -650,48 +635,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -707,35 +650,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -746,6 +662,114 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1079,7 +1103,7 @@
   <dimension ref="A1:S48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1105,7 +1129,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="15.75" thickBot="1">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="23" t="s">
         <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1143,23 +1167,23 @@
       </c>
     </row>
     <row r="2" spans="2:19" ht="15.75" thickBot="1">
-      <c r="B2" s="28">
+      <c r="B2" s="59">
         <v>0</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="60">
         <v>1.8</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="61">
         <v>705</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="62">
         <v>144</v>
       </c>
-      <c r="G2" s="18">
+      <c r="G2" s="63">
         <v>0</v>
       </c>
       <c r="I2" s="15">
-        <f>D2*IF(B2=0,(360/C2),B2)*64</f>
+        <f>ROUND(D2*IF(B2=0,(360/C2),B2)*64,0)</f>
         <v>9024000</v>
       </c>
       <c r="J2" s="13">
@@ -1174,7 +1198,7 @@
         <v>62667</v>
       </c>
       <c r="M2" s="15">
-        <f>IF(G2=0,ROUNDUP(I2/10000000,0),IF(G2&lt;ROUNDUP(I2/10000000,0),ROUNDUP(I2/10000000,0),G2))</f>
+        <f>MAX(IF(G2=0,ROUNDUP(I2/10000000,0),IF(G2&lt;ROUNDUP(I2/10000000,0),ROUNDUP(I2/10000000,0),G2)),IF(G2=0,ROUNDUP(I23/10000000,0),IF(G2&lt;ROUNDUP(I23/10000000,0),ROUNDUP(I23/10000000,0),G2)))</f>
         <v>1</v>
       </c>
       <c r="N2" s="13">
@@ -1186,46 +1210,46 @@
       </c>
     </row>
     <row r="3" spans="2:19" ht="15" customHeight="1">
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="G3" s="42" t="s">
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="G3" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="46" t="s">
+      <c r="I3" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
-      <c r="O3" s="46"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42"/>
     </row>
     <row r="4" spans="2:19" ht="15.75" thickBot="1">
-      <c r="B4" s="34"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="G4" s="43"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="46"/>
-      <c r="N4" s="46"/>
-      <c r="O4" s="46"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="G4" s="48"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="42"/>
       <c r="P4" s="9"/>
       <c r="Q4" s="9"/>
       <c r="R4" s="9"/>
     </row>
     <row r="5" spans="2:19" ht="15.75" hidden="1" customHeight="1">
-      <c r="B5" s="34"/>
+      <c r="B5" s="44"/>
       <c r="I5">
         <f>K2</f>
         <v>64933</v>
@@ -1235,7 +1259,7 @@
       </c>
     </row>
     <row r="6" spans="2:19" ht="15.75" hidden="1" customHeight="1">
-      <c r="B6" s="34"/>
+      <c r="B6" s="44"/>
       <c r="I6">
         <f>N2*O2</f>
         <v>124000000</v>
@@ -1257,7 +1281,7 @@
       </c>
     </row>
     <row r="7" spans="2:19" ht="15.75" hidden="1" customHeight="1">
-      <c r="B7" s="34"/>
+      <c r="B7" s="44"/>
       <c r="I7" t="s">
         <v>19</v>
       </c>
@@ -1278,7 +1302,7 @@
       </c>
     </row>
     <row r="8" spans="2:19" ht="15.75" hidden="1" customHeight="1">
-      <c r="B8" s="34"/>
+      <c r="B8" s="44"/>
       <c r="I8" t="str">
         <f>CONCATENATE(" ",I2,",")</f>
         <v xml:space="preserve"> 9024000,</v>
@@ -1304,86 +1328,86 @@
       </c>
     </row>
     <row r="9" spans="2:19" ht="15.75" hidden="1" customHeight="1">
-      <c r="B9" s="34"/>
+      <c r="B9" s="44"/>
       <c r="I9" s="2" t="str">
         <f>CONCATENATE(" ",K2,",")</f>
         <v xml:space="preserve"> 64933,</v>
       </c>
     </row>
     <row r="10" spans="2:19" ht="15.75" hidden="1" customHeight="1">
-      <c r="B10" s="34"/>
+      <c r="B10" s="44"/>
       <c r="I10" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:19" ht="15.75" hidden="1" customHeight="1">
-      <c r="B11" s="34"/>
+      <c r="B11" s="44"/>
       <c r="I11" s="2" t="str">
         <f>CONCATENATE(" ",L2,",")</f>
         <v xml:space="preserve"> 62667,</v>
       </c>
     </row>
     <row r="12" spans="2:19" ht="15.75" hidden="1" customHeight="1" thickBot="1">
-      <c r="B12" s="34"/>
+      <c r="B12" s="44"/>
       <c r="I12" s="2" t="str">
         <f>CONCATENATE(" ",M2,");")</f>
         <v xml:space="preserve"> 1);</v>
       </c>
     </row>
     <row r="13" spans="2:19" s="9" customFormat="1" ht="15" customHeight="1">
-      <c r="B13" s="34"/>
-      <c r="C13" s="37" t="s">
+      <c r="B13" s="44"/>
+      <c r="C13" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="37"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="36" t="str">
+      <c r="D13" s="49"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="65" t="str">
         <f>IF(E16,CONCATENATE("Synta synta(",I7,I8,I29,I9,I30,I11,I31,I10,I12),CONCATENATE("Synta synta(",I7,I8,I9,I10,I11,I12))</f>
         <v>Synta synta(1281, 9024000, 64933, 16, 62667, 1);</v>
       </c>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="37"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="38"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="66"/>
+      <c r="L13" s="66"/>
+      <c r="M13" s="66"/>
+      <c r="N13" s="66"/>
+      <c r="O13" s="67"/>
     </row>
     <row r="14" spans="2:19" ht="15.75" thickBot="1">
-      <c r="B14" s="34"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="40"/>
-      <c r="L14" s="40"/>
-      <c r="M14" s="40"/>
-      <c r="N14" s="40"/>
-      <c r="O14" s="41"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="68"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="69"/>
+      <c r="J14" s="69"/>
+      <c r="K14" s="69"/>
+      <c r="L14" s="69"/>
+      <c r="M14" s="69"/>
+      <c r="N14" s="69"/>
+      <c r="O14" s="70"/>
     </row>
     <row r="15" spans="2:19" ht="15.75" thickBot="1">
-      <c r="B15" s="34"/>
+      <c r="B15" s="44"/>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="2:19" ht="15.75" thickBot="1">
-      <c r="B16" s="34"/>
+      <c r="B16" s="44"/>
       <c r="C16" s="53" t="s">
         <v>34</v>
       </c>
       <c r="D16" s="54"/>
-      <c r="E16" s="59">
+      <c r="E16" s="64">
         <v>0</v>
       </c>
-      <c r="G16" s="25" t="s">
+      <c r="G16" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="H16" s="20" t="s">
+      <c r="H16" s="17" t="s">
         <v>20</v>
       </c>
       <c r="I16" s="4" t="s">
@@ -1400,16 +1424,16 @@
       </c>
     </row>
     <row r="17" spans="2:18">
-      <c r="B17" s="52"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="55" t="s">
         <v>35</v>
       </c>
       <c r="D17" s="56"/>
       <c r="E17" s="56"/>
-      <c r="G17" s="23" t="s">
+      <c r="G17" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="22"/>
+      <c r="H17" s="19"/>
       <c r="I17">
         <f>(Q6*64 + S7)/64</f>
         <v>19096.59375</v>
@@ -1428,14 +1452,14 @@
       </c>
     </row>
     <row r="18" spans="2:18">
-      <c r="B18" s="34"/>
+      <c r="B18" s="44"/>
       <c r="C18" s="57"/>
       <c r="D18" s="58"/>
       <c r="E18" s="58"/>
-      <c r="G18" s="24" t="s">
+      <c r="G18" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="H18" s="21"/>
+      <c r="H18" s="18"/>
       <c r="I18">
         <f>Q6</f>
         <v>19096</v>
@@ -1454,47 +1478,47 @@
       </c>
     </row>
     <row r="19" spans="2:18">
-      <c r="B19" s="35"/>
+      <c r="B19" s="45"/>
       <c r="C19" s="57"/>
       <c r="D19" s="58"/>
       <c r="E19" s="58"/>
     </row>
     <row r="20" spans="2:18">
-      <c r="B20" s="51"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51"/>
-      <c r="G20" s="51"/>
-      <c r="H20" s="51"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="51"/>
-      <c r="K20" s="51"/>
-      <c r="L20" s="51"/>
-      <c r="M20" s="51"/>
-      <c r="N20" s="51"/>
-      <c r="O20" s="51"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="32"/>
+      <c r="O20" s="32"/>
     </row>
     <row r="21" spans="2:18" ht="15.75" thickBot="1">
-      <c r="B21" s="61" t="s">
+      <c r="B21" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="61"/>
-      <c r="D21" s="61"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="61"/>
-      <c r="H21" s="61"/>
-      <c r="I21" s="61"/>
-      <c r="J21" s="61"/>
-      <c r="K21" s="61"/>
-      <c r="L21" s="61"/>
-      <c r="M21" s="61"/>
-      <c r="N21" s="61"/>
-      <c r="O21" s="61"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="39"/>
     </row>
     <row r="22" spans="2:18" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B22" s="60" t="s">
+      <c r="B22" s="33" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -1506,7 +1530,7 @@
       <c r="E22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="47"/>
+      <c r="G22" s="28"/>
       <c r="I22" s="10" t="s">
         <v>29</v>
       </c>
@@ -1528,21 +1552,21 @@
       </c>
     </row>
     <row r="23" spans="2:18" ht="15.75" thickBot="1">
-      <c r="B23" s="28">
+      <c r="B23" s="59">
         <v>0</v>
       </c>
-      <c r="C23" s="26">
+      <c r="C23" s="60">
         <v>1.8</v>
       </c>
-      <c r="D23" s="16">
+      <c r="D23" s="61">
         <v>705</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E23" s="62">
         <v>144</v>
       </c>
-      <c r="G23" s="48"/>
+      <c r="G23" s="29"/>
       <c r="I23" s="15">
-        <f>D23*IF(B23=0,(360/C23),B23)*64</f>
+        <f>ROUND(D23*IF(B23=0,(360/C23),B23)*64,0)</f>
         <v>9024000</v>
       </c>
       <c r="J23" s="13">
@@ -1556,7 +1580,7 @@
         <f>ROUND(I23/E23,0)</f>
         <v>62667</v>
       </c>
-      <c r="M23" s="49"/>
+      <c r="M23" s="30"/>
       <c r="N23" s="13">
         <v>620</v>
       </c>
@@ -1566,52 +1590,52 @@
       </c>
     </row>
     <row r="24" spans="2:18" ht="15" customHeight="1">
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="44" t="s">
+      <c r="C24" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
-      <c r="G24" s="31"/>
-      <c r="I24" s="46" t="s">
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="G24" s="26"/>
+      <c r="I24" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="J24" s="46"/>
-      <c r="K24" s="46"/>
-      <c r="L24" s="46"/>
-      <c r="M24" s="46"/>
-      <c r="N24" s="46"/>
-      <c r="O24" s="46"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="42"/>
     </row>
     <row r="25" spans="2:18">
-      <c r="B25" s="34"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
-      <c r="G25" s="31"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="46"/>
-      <c r="L25" s="46"/>
-      <c r="M25" s="46"/>
-      <c r="N25" s="46"/>
-      <c r="O25" s="46"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
+      <c r="G25" s="26"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="42"/>
       <c r="P25" s="9"/>
       <c r="Q25" s="9"/>
     </row>
     <row r="26" spans="2:18" ht="15" hidden="1" customHeight="1">
-      <c r="B26" s="34"/>
+      <c r="B26" s="44"/>
     </row>
     <row r="27" spans="2:18" ht="15" hidden="1" customHeight="1">
-      <c r="B27" s="34"/>
+      <c r="B27" s="44"/>
     </row>
     <row r="28" spans="2:18" ht="15" hidden="1" customHeight="1">
-      <c r="B28" s="34"/>
+      <c r="B28" s="44"/>
     </row>
     <row r="29" spans="2:18" ht="15" hidden="1" customHeight="1">
-      <c r="B29" s="34"/>
+      <c r="B29" s="44"/>
       <c r="I29" t="str">
         <f>CONCATENATE(" ",I23,",")</f>
         <v xml:space="preserve"> 9024000,</v>
@@ -1621,160 +1645,160 @@
       </c>
     </row>
     <row r="30" spans="2:18" ht="15" hidden="1" customHeight="1">
-      <c r="B30" s="34"/>
+      <c r="B30" s="44"/>
       <c r="I30" s="2" t="str">
         <f>CONCATENATE(" ",K23,",")</f>
         <v xml:space="preserve"> 64933,</v>
       </c>
-      <c r="J30" s="50"/>
-      <c r="K30" s="50"/>
-      <c r="L30" s="50"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
-      <c r="O30" s="19"/>
+      <c r="J30" s="31"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="31"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
       <c r="P30" s="9"/>
       <c r="Q30" s="9"/>
     </row>
     <row r="31" spans="2:18" ht="15" hidden="1" customHeight="1">
-      <c r="B31" s="34"/>
+      <c r="B31" s="44"/>
       <c r="I31" s="2" t="str">
         <f>CONCATENATE(" ",L23,",")</f>
         <v xml:space="preserve"> 62667,</v>
       </c>
-      <c r="J31" s="50"/>
-      <c r="K31" s="50"/>
-      <c r="L31" s="50"/>
-      <c r="M31" s="19"/>
-      <c r="N31" s="19"/>
-      <c r="O31" s="19"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="31"/>
+      <c r="L31" s="31"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
     </row>
     <row r="32" spans="2:18" ht="15" hidden="1" customHeight="1">
-      <c r="B32" s="34"/>
+      <c r="B32" s="44"/>
     </row>
     <row r="33" spans="1:15" ht="15" hidden="1" customHeight="1">
-      <c r="B33" s="34"/>
+      <c r="B33" s="44"/>
       <c r="I33" s="2"/>
-      <c r="J33" s="47"/>
-      <c r="K33" s="47"/>
-      <c r="L33" s="47"/>
-      <c r="M33" s="32"/>
-      <c r="N33" s="32"/>
-      <c r="O33" s="32"/>
+      <c r="J33" s="28"/>
+      <c r="K33" s="28"/>
+      <c r="L33" s="28"/>
+      <c r="M33" s="27"/>
+      <c r="N33" s="27"/>
+      <c r="O33" s="27"/>
     </row>
     <row r="34" spans="1:15" ht="15" hidden="1" customHeight="1">
       <c r="A34" s="9"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="50"/>
-      <c r="D34" s="50"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="50"/>
-      <c r="G34" s="50"/>
-      <c r="H34" s="50"/>
-      <c r="I34" s="50"/>
-      <c r="J34" s="65"/>
-      <c r="K34" s="65"/>
-      <c r="L34" s="66"/>
-      <c r="M34" s="32"/>
-      <c r="N34" s="32"/>
-      <c r="O34" s="32"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="37"/>
+      <c r="L34" s="38"/>
+      <c r="M34" s="27"/>
+      <c r="N34" s="27"/>
+      <c r="O34" s="27"/>
     </row>
     <row r="35" spans="1:15" ht="15" hidden="1" customHeight="1">
-      <c r="B35" s="34"/>
-      <c r="C35" s="50"/>
-      <c r="D35" s="50"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="50"/>
-      <c r="I35" s="50"/>
-      <c r="J35" s="65"/>
-      <c r="K35" s="65"/>
-      <c r="L35" s="66"/>
-      <c r="M35" s="32"/>
-      <c r="N35" s="32"/>
-      <c r="O35" s="32"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="37"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="38"/>
+      <c r="M35" s="27"/>
+      <c r="N35" s="27"/>
+      <c r="O35" s="27"/>
     </row>
     <row r="36" spans="1:15" ht="15" hidden="1" customHeight="1">
-      <c r="B36" s="34"/>
+      <c r="B36" s="44"/>
       <c r="I36" s="2"/>
-      <c r="J36" s="32"/>
-      <c r="K36" s="32"/>
-      <c r="L36" s="32"/>
-      <c r="M36" s="32"/>
-      <c r="N36" s="32"/>
-      <c r="O36" s="32"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="27"/>
+      <c r="L36" s="27"/>
+      <c r="M36" s="27"/>
+      <c r="N36" s="27"/>
+      <c r="O36" s="27"/>
     </row>
     <row r="37" spans="1:15" hidden="1">
-      <c r="B37" s="34"/>
-      <c r="G37" s="62"/>
-      <c r="H37" s="63"/>
-      <c r="I37" s="47"/>
-      <c r="J37" s="32"/>
-      <c r="K37" s="32"/>
-      <c r="L37" s="32"/>
-      <c r="M37" s="32"/>
-      <c r="N37" s="32"/>
-      <c r="O37" s="32"/>
+      <c r="B37" s="44"/>
+      <c r="G37" s="34"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="28"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="27"/>
+      <c r="L37" s="27"/>
+      <c r="M37" s="27"/>
+      <c r="N37" s="27"/>
+      <c r="O37" s="27"/>
     </row>
     <row r="38" spans="1:15">
-      <c r="B38" s="34"/>
-      <c r="G38" s="64"/>
-      <c r="H38" s="64"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="32"/>
-      <c r="K38" s="32"/>
-      <c r="L38" s="32"/>
-      <c r="M38" s="32"/>
-      <c r="N38" s="32"/>
-      <c r="O38" s="32"/>
+      <c r="B38" s="44"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="27"/>
+      <c r="L38" s="27"/>
+      <c r="M38" s="27"/>
+      <c r="N38" s="27"/>
+      <c r="O38" s="27"/>
     </row>
     <row r="39" spans="1:15">
-      <c r="B39" s="34"/>
-      <c r="G39" s="64"/>
-      <c r="H39" s="64"/>
-      <c r="I39" s="32"/>
-      <c r="J39" s="32"/>
-      <c r="K39" s="32"/>
-      <c r="L39" s="32"/>
-      <c r="M39" s="32"/>
-      <c r="N39" s="32"/>
-      <c r="O39" s="32"/>
+      <c r="B39" s="44"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="36"/>
+      <c r="I39" s="27"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="27"/>
+      <c r="L39" s="27"/>
+      <c r="M39" s="27"/>
+      <c r="N39" s="27"/>
+      <c r="O39" s="27"/>
     </row>
     <row r="40" spans="1:15">
-      <c r="B40" s="34"/>
-      <c r="G40" s="32"/>
-      <c r="H40" s="32"/>
-      <c r="I40" s="32"/>
-      <c r="J40" s="32"/>
-      <c r="K40" s="32"/>
-      <c r="L40" s="32"/>
-      <c r="M40" s="32"/>
-      <c r="N40" s="32"/>
-      <c r="O40" s="32"/>
+      <c r="B40" s="44"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="27"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="27"/>
+      <c r="L40" s="27"/>
+      <c r="M40" s="27"/>
+      <c r="N40" s="27"/>
+      <c r="O40" s="27"/>
     </row>
     <row r="41" spans="1:15">
-      <c r="B41" s="34"/>
-      <c r="G41" s="32"/>
-      <c r="H41" s="32"/>
-      <c r="I41" s="32"/>
+      <c r="B41" s="44"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="27"/>
     </row>
     <row r="42" spans="1:15">
-      <c r="B42" s="34"/>
-      <c r="G42" s="32"/>
-      <c r="H42" s="32"/>
-      <c r="I42" s="32"/>
+      <c r="B42" s="44"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="27"/>
+      <c r="I42" s="27"/>
     </row>
     <row r="43" spans="1:15">
-      <c r="B43" s="34"/>
-      <c r="G43" s="32"/>
-      <c r="H43" s="32"/>
-      <c r="I43" s="32"/>
+      <c r="B43" s="44"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
     </row>
     <row r="44" spans="1:15">
-      <c r="B44" s="35"/>
-      <c r="G44" s="32"/>
-      <c r="H44" s="32"/>
-      <c r="I44" s="32"/>
+      <c r="B44" s="45"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
     </row>
     <row r="48" spans="1:15">
       <c r="G48" t="s">
@@ -1782,6 +1806,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection password="F6F4" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="12">
     <mergeCell ref="B21:O21"/>
     <mergeCell ref="C24:E25"/>
@@ -1808,7 +1833,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>

</xml_diff>